<commit_message>
update the function of leaderboard
</commit_message>
<xml_diff>
--- a/server/final_dummy_data_with_names (1).xlsx
+++ b/server/final_dummy_data_with_names (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dowanload2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mostafa\Documents\GitHub\Sanabel_Al-Ehsan\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD0266B-B5B7-4E05-8978-2167EE1B07DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F335F4E-FFC0-41EE-B11A-77CF2B635B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="2964" windowWidth="17064" windowHeight="8688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Genre</t>
-  </si>
-  <si>
     <t>DateOfBirth</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>tamer</t>
+  </si>
+  <si>
+    <t>Gendre</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,305 +627,305 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" t="s">
         <v>62</v>
-      </c>
-      <c r="H9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
         <v>62</v>
-      </c>
-      <c r="H10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>